<commit_message>
load list student UI
</commit_message>
<xml_diff>
--- a/ManageStudents/out/production/ManageStudents/Data/managestudents.xlsx
+++ b/ManageStudents/out/production/ManageStudents/Data/managestudents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\Project\github\ManageStudents\ManageStudents\src\DataCSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\Project\github\ManageStudents\ManageStudents\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C835917-70B0-4B16-9940-F77521F5F808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0760145D-29BD-42AA-8146-A4A4B4934A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t xml:space="preserve">Nguyễn Văn A </t>
   </si>
@@ -245,6 +245,39 @@
   </si>
   <si>
     <t>C43</t>
+  </si>
+  <si>
+    <t>Subject Id</t>
+  </si>
+  <si>
+    <t>Subject Name</t>
+  </si>
+  <si>
+    <t>Class Id</t>
+  </si>
+  <si>
+    <t>Subject ID</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Mssv</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Cmnd</t>
+  </si>
+  <si>
+    <t>ClassId</t>
+  </si>
+  <si>
+    <t>Class Name</t>
   </si>
 </sst>
 </file>
@@ -1085,43 +1118,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1742001</v>
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>123456789</v>
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1742002</v>
+        <v>1742001</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>123456788</v>
+        <v>123456789</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
@@ -1129,16 +1166,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1742003</v>
+        <v>1742002</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>123456787</v>
+        <v>123456788</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -1146,16 +1183,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1742004</v>
+        <v>1742003</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>123456786</v>
+        <v>123456787</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
@@ -1163,16 +1200,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>1742005</v>
+        <v>1742004</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>123456785</v>
+        <v>123456786</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
@@ -1180,16 +1217,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>1742006</v>
+        <v>1742005</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>123456749</v>
+        <v>123456785</v>
       </c>
       <c r="E6" t="s">
         <v>38</v>
@@ -1197,16 +1234,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1742007</v>
+        <v>1742006</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>123456739</v>
+        <v>123456749</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
@@ -1214,33 +1251,33 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>1742008</v>
+        <v>1742007</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>123456289</v>
+        <v>123456739</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>1742009</v>
+        <v>1742008</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>123156789</v>
+        <v>123456289</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -1248,16 +1285,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1742010</v>
+        <v>1742009</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>123459789</v>
+        <v>123156789</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -1265,16 +1302,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1742011</v>
+        <v>1742010</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>123453789</v>
+        <v>123459789</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1282,16 +1319,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1742012</v>
+        <v>1742011</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>123452789</v>
+        <v>123453789</v>
       </c>
       <c r="E12" t="s">
         <v>39</v>
@@ -1299,16 +1336,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>1742013</v>
+        <v>1742012</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13">
-        <v>123416789</v>
+        <v>123452789</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -1316,16 +1353,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>1742014</v>
+        <v>1742013</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>127456789</v>
+        <v>123416789</v>
       </c>
       <c r="E14" t="s">
         <v>39</v>
@@ -1333,16 +1370,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>1742015</v>
+        <v>1742014</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>123456769</v>
+        <v>127456789</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
@@ -1350,16 +1387,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>1742016</v>
+        <v>1742015</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16">
-        <v>123456789</v>
+        <v>123456769</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -1367,16 +1404,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>1742017</v>
+        <v>1742016</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17">
-        <v>123416789</v>
+        <v>123456789</v>
       </c>
       <c r="E17" t="s">
         <v>39</v>
@@ -1384,33 +1421,33 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>1742018</v>
+        <v>1742017</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18">
-        <v>923456789</v>
+        <v>123416789</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>1742019</v>
+        <v>1742018</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19">
-        <v>823456789</v>
+        <v>923456789</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1418,16 +1455,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>1742020</v>
+        <v>1742019</v>
       </c>
       <c r="C20" t="s">
         <v>13</v>
       </c>
       <c r="D20">
-        <v>723456789</v>
+        <v>823456789</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
@@ -1435,16 +1472,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>1742021</v>
+        <v>1742020</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
       </c>
       <c r="D21">
-        <v>623456789</v>
+        <v>723456789</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -1452,16 +1489,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>1742022</v>
+        <v>1742021</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
       </c>
       <c r="D22">
-        <v>523456789</v>
+        <v>623456789</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -1469,16 +1506,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>1742023</v>
+        <v>1742022</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23">
-        <v>423456789</v>
+        <v>523456789</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -1486,16 +1523,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>1742024</v>
+        <v>1742023</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="D24">
-        <v>323456789</v>
+        <v>423456789</v>
       </c>
       <c r="E24" t="s">
         <v>40</v>
@@ -1503,16 +1540,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>1742025</v>
+        <v>1742024</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25">
-        <v>223456789</v>
+        <v>323456789</v>
       </c>
       <c r="E25" t="s">
         <v>40</v>
@@ -1520,16 +1557,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>1742026</v>
+        <v>1742025</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26">
-        <v>123456749</v>
+        <v>223456789</v>
       </c>
       <c r="E26" t="s">
         <v>40</v>
@@ -1537,16 +1574,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>1742027</v>
+        <v>1742026</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
       </c>
       <c r="D27">
-        <v>123456739</v>
+        <v>123456749</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
@@ -1554,16 +1591,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>1742028</v>
+        <v>1742027</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>123456729</v>
+        <v>123456739</v>
       </c>
       <c r="E28" t="s">
         <v>40</v>
@@ -1571,33 +1608,33 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>1742029</v>
+        <v>1742028</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>123456719</v>
+        <v>123456729</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>1742030</v>
+        <v>1742029</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>123456989</v>
+        <v>123456719</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1605,16 +1642,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>1742031</v>
+        <v>1742030</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>123456889</v>
+        <v>123456989</v>
       </c>
       <c r="E31" t="s">
         <v>41</v>
@@ -1622,16 +1659,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>1742032</v>
+        <v>1742031</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>123456789</v>
+        <v>123456889</v>
       </c>
       <c r="E32" t="s">
         <v>41</v>
@@ -1639,16 +1676,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>1742033</v>
+        <v>1742032</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>12345689</v>
+        <v>123456789</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1656,16 +1693,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>1742034</v>
+        <v>1742033</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>1234156789</v>
+        <v>12345689</v>
       </c>
       <c r="E34" t="s">
         <v>41</v>
@@ -1673,16 +1710,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>1742035</v>
+        <v>1742034</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>123556789</v>
+        <v>1234156789</v>
       </c>
       <c r="E35" t="s">
         <v>41</v>
@@ -1690,18 +1727,35 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
-        <v>1742036</v>
+        <v>1742035</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
       <c r="D36">
+        <v>123556789</v>
+      </c>
+      <c r="E36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>1742036</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37">
         <v>123456589</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1712,43 +1766,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1759,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1772,81 +1834,89 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1857,23 +1927,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1881,10 +1951,10 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1892,10 +1962,10 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1903,21 +1973,21 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1925,10 +1995,10 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1936,10 +2006,10 @@
         <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1947,21 +2017,21 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1969,10 +2039,10 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1980,21 +2050,21 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2002,10 +2072,10 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2013,9 +2083,20 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>